<commit_message>
update of requirements table - not finished
</commit_message>
<xml_diff>
--- a/part A/טבלת_דרישות_מערכת_לניהול_קופונים.xlsx
+++ b/part A/טבלת_דרישות_מערכת_לניהול_קופונים.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="141">
   <si>
     <t>תאור הדרישה</t>
   </si>
@@ -401,26 +401,59 @@
     <t>משתמשים בעלי עסק יכולים לצפות בכל עת בהזמנות של הקופונים שלהם.</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>nf</t>
-  </si>
-  <si>
-    <t>f**</t>
-  </si>
-  <si>
-    <t>nf*</t>
-  </si>
-  <si>
-    <t>f*</t>
+    <t>פונקציונלית</t>
+  </si>
+  <si>
+    <t>לא פונקציונלית</t>
+  </si>
+  <si>
+    <t>בעת הוספת משתמש, המערכת תדרוש פרטי זיהוי (שם משתמש, מייל, טלפון).</t>
+  </si>
+  <si>
+    <t>בעת הוספת משתמש, המערכת תדרוש סיסמא חזקה</t>
+  </si>
+  <si>
+    <t>פונקציולית</t>
+  </si>
+  <si>
+    <t>מפוצל</t>
+  </si>
+  <si>
+    <t>3.1.2.1</t>
+  </si>
+  <si>
+    <t>3.1.2.2</t>
+  </si>
+  <si>
+    <t>4.1.1.1</t>
+  </si>
+  <si>
+    <t>4.1.1.2</t>
+  </si>
+  <si>
+    <t>המערכת תתמוך בהזמנת קופונים מבתי עסק.</t>
+  </si>
+  <si>
+    <t>הזמנת קופונים תתאפשר ע"י משתמשים רשומים במערכת.</t>
+  </si>
+  <si>
+    <t>אורי</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>אבירם</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,8 +494,22 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,12 +518,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -484,25 +543,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -625,15 +726,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G41" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <tableColumns count="7">
-    <tableColumn id="1" name="מס&quot;ד" dataDxfId="6"/>
-    <tableColumn id="2" name="קבוצת תהליך" dataDxfId="5"/>
-    <tableColumn id="3" name="תהליך" dataDxfId="4"/>
-    <tableColumn id="4" name="תאור הדרישה" dataDxfId="3"/>
-    <tableColumn id="5" name="מקור הדרישה" dataDxfId="2"/>
-    <tableColumn id="6" name="סוג" dataDxfId="1"/>
-    <tableColumn id="7" name="עדיפות" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I46" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <tableColumns count="9">
+    <tableColumn id="1" name="מס&quot;ד" dataDxfId="8"/>
+    <tableColumn id="2" name="קבוצת תהליך" dataDxfId="7"/>
+    <tableColumn id="3" name="תהליך" dataDxfId="6"/>
+    <tableColumn id="4" name="תאור הדרישה" dataDxfId="5"/>
+    <tableColumn id="5" name="מקור הדרישה" dataDxfId="4"/>
+    <tableColumn id="6" name="סוג" dataDxfId="3"/>
+    <tableColumn id="7" name="עדיפות" dataDxfId="2"/>
+    <tableColumn id="8" name="Column1" dataDxfId="1"/>
+    <tableColumn id="9" name="Column2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -902,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -913,13 +1016,13 @@
     <col min="1" max="1" width="9.375" customWidth="1"/>
     <col min="2" max="2" width="21.875" customWidth="1"/>
     <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.5" customWidth="1"/>
-    <col min="5" max="5" width="19.125" customWidth="1"/>
+    <col min="4" max="4" width="52.875" customWidth="1"/>
+    <col min="5" max="5" width="9.875" customWidth="1"/>
     <col min="6" max="6" width="14.25" customWidth="1"/>
     <col min="7" max="7" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -941,8 +1044,14 @@
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H1" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -950,8 +1059,10 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>100</v>
       </c>
@@ -973,8 +1084,10 @@
       <c r="G3" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -982,8 +1095,10 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -1005,8 +1120,10 @@
       <c r="G5" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>51</v>
       </c>
@@ -1023,13 +1140,15 @@
         <v>85</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>52</v>
       </c>
@@ -1051,8 +1170,10 @@
       <c r="G7" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
@@ -1074,8 +1195,10 @@
       <c r="G8" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -1085,7 +1208,7 @@
       <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1097,8 +1220,10 @@
       <c r="G9" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>55</v>
       </c>
@@ -1108,20 +1233,22 @@
       <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="5" t="s">
         <v>126</v>
       </c>
       <c r="G10" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>56</v>
       </c>
@@ -1143,8 +1270,10 @@
       <c r="G11" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>102</v>
       </c>
@@ -1166,8 +1295,10 @@
       <c r="G12" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>103</v>
       </c>
@@ -1177,7 +1308,7 @@
       <c r="C13" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="6" t="s">
         <v>105</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1189,8 +1320,10 @@
       <c r="G13" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>106</v>
       </c>
@@ -1200,7 +1333,7 @@
       <c r="C14" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1212,33 +1345,23 @@
       <c r="G14" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G15" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>9</v>
@@ -1247,44 +1370,48 @@
         <v>19</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>85</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G16" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>125</v>
+      <c r="F17" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="G17" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>9</v>
@@ -1293,21 +1420,23 @@
         <v>20</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>115</v>
+        <v>22</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="7" t="s">
         <v>125</v>
       </c>
       <c r="G18" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>9</v>
@@ -1316,99 +1445,109 @@
         <v>20</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="7" t="s">
         <v>125</v>
       </c>
       <c r="G19" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>126</v>
+      <c r="F20" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="G20" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="7" t="s">
         <v>126</v>
       </c>
       <c r="G21" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" s="3">
+        <v>4</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G23" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>10</v>
@@ -1417,21 +1556,27 @@
         <v>14</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>128</v>
+      <c r="F24" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="G24" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H24" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>10</v>
@@ -1439,22 +1584,24 @@
       <c r="C25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>24</v>
+      <c r="D25" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>128</v>
+      <c r="F25" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="G25" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>65</v>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>10</v>
@@ -1462,215 +1609,231 @@
       <c r="C26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G26" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>66</v>
+      <c r="D26" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G26" s="7">
+        <v>5</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="3">
+        <v>14</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G27" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>120</v>
+        <v>24</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>128</v>
+        <v>85</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="G28" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="7" t="s">
         <v>125</v>
       </c>
       <c r="G29" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="8" t="s">
         <v>125</v>
       </c>
       <c r="G30" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>38</v>
+        <v>120</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>128</v>
+      <c r="F31" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="G31" s="3">
+        <v>3</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G32" s="3">
+        <v>5</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G33" s="3">
+        <v>3</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G34" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G33" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="G34" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="G35" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>11</v>
@@ -1678,321 +1841,371 @@
       <c r="C36" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>121</v>
+      <c r="D36" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>125</v>
+        <v>85</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>130</v>
       </c>
       <c r="G36" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>75</v>
+        <v>5</v>
+      </c>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>49</v>
+        <v>27</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>129</v>
+        <v>85</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="G37" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>110</v>
+        <v>5</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>111</v>
+        <v>27</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F38" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" s="7" t="s">
         <v>126</v>
       </c>
       <c r="G38" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>94</v>
+      <c r="C39" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>125</v>
+      <c r="F39" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="G39" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>125</v>
+        <v>86</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="G40" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G41" s="3">
+        <v>4</v>
+      </c>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+    </row>
+    <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>36</v>
+        <v>48</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>125</v>
       </c>
       <c r="G42" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>112</v>
+        <v>48</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F43" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" s="10" t="s">
         <v>125</v>
       </c>
       <c r="G43" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+    </row>
+    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G44" s="3">
+        <v>2</v>
+      </c>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+    </row>
+    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G45" s="3">
+        <v>4</v>
+      </c>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G44" s="3">
+      <c r="D47" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G47" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G48" s="3">
         <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G45" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G46" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-    </row>
-    <row r="48" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G48" s="3">
-        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>124</v>
+        <v>18</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F49" s="4" t="s">
         <v>125</v>
       </c>
       <c r="G49" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>43</v>
+        <v>18</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F50" s="4" t="s">
         <v>125</v>
       </c>
       <c r="G50" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
@@ -2004,31 +2217,73 @@
       <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
+      <c r="A53" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G53" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
+      <c r="A54" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G54" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
+      <c r="A55" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G55" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
@@ -2102,9 +2357,54 @@
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
     </row>
+    <row r="64" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+    </row>
+    <row r="66" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>